<commit_message>
create /trans and keboard and edit excel_parser.py
</commit_message>
<xml_diff>
--- a/pathxl/680009374.xlsx
+++ b/pathxl/680009374.xlsx
@@ -2,14 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -49,7 +50,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -412,159 +413,149 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A23"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="n">
-        <v>1</v>
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>cat</t>
+        </is>
+      </c>
+      <c r="B1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <f>IF(B1&lt;&gt;1,A1,)</f>
+        <v/>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>2</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>dog</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <f>IF(B2&lt;&gt;1,A2,)</f>
+        <v/>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>brown</t>
-        </is>
+          <t>mouse</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <f>IF(B3&lt;&gt;1,A3,)</f>
+        <v/>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>lock</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <f>IF(B4&lt;&gt;1,A4,)</f>
+        <v/>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>hourse</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <f>IF(B5&lt;&gt;1,A5,)</f>
+        <v/>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>mouse</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <f>IF(B6&lt;&gt;1,A6,)</f>
+        <v/>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>click</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <f>IF(B7&lt;&gt;1,A7,)</f>
+        <v/>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
-        <v>7</v>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>damn</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <f>IF(B8&lt;&gt;1,A8,)</f>
+        <v/>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>yoga</t>
-        </is>
+          <t>damp</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <f>IF(B9&lt;&gt;1,A9,)</f>
+        <v/>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>park</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>cross</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>bear</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>mouse</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>micro</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>abracadabra</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>mm</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>you</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>go</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>do</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>dude</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>bro</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>babe</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>done</t>
-        </is>
+          <t>clock</t>
+        </is>
+      </c>
+      <c r="C10">
+        <f>IF(B10&lt;&gt;1,A10,)</f>
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>